<commit_message>
experiment with local news
</commit_message>
<xml_diff>
--- a/cleaned_goldendata_extracted_feature.xlsx
+++ b/cleaned_goldendata_extracted_feature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github Repository\ta-newsX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341BC1EB-C552-42EB-A0AC-49E0D7FA1E30}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7E9F2A-F199-4F7C-B697-1416529E6E11}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2977,10 +2977,10 @@
   <dimension ref="A1:H1616"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B1475" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B1246" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1:G1048576"/>
+      <selection pane="bottomRight" activeCell="F1224" sqref="F1224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2989,7 +2989,7 @@
     <col min="2" max="2" width="5.54296875" customWidth="1"/>
     <col min="3" max="3" width="16" style="7" customWidth="1"/>
     <col min="6" max="6" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.453125" style="9" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7265625" style="9" customWidth="1"/>
     <col min="8" max="8" width="8.7265625" style="9"/>
   </cols>
   <sheetData>

</xml_diff>